<commit_message>
GeneRiskChart: add make and female options, and made some cosmetic changes to the layout
</commit_message>
<xml_diff>
--- a/data-graph-MUSC/MASTER_RiskTo85ForGraph.xlsx
+++ b/data-graph-MUSC/MASTER_RiskTo85ForGraph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keh270\Dropbox\StudentsResearchAssociates\TablesForJulie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zach/src/_-MUSC/graph-musc/data-graph-MUSC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E2ED7B-68B4-48D5-A2B9-3A2765DBF654}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF82CFB4-A459-9748-8F03-3F6F14BC4A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="500" windowWidth="23900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER_RiskTo85ForGraph" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Wrong_MASTER_RiskTo85ForGraph" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MASTER_RiskTo85ForGraph!$A$1:$E$180</definedName>
     <definedName name="MASTER_RiskTo85ForGraph">Wrong_MASTER_RiskTo85ForGraph!$A$1:$E$172</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -704,11 +705,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -773,10 +776,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1118,15 +1121,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5417913A-0891-445A-91B9-26EAB1278E71}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>213</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1160,7 +1162,7 @@
         <v>39.61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1177,7 +1179,7 @@
         <v>8.34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1194,7 +1196,7 @@
         <v>7.08</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1228,7 +1230,7 @@
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1245,7 +1247,7 @@
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1264,7 @@
         <v>4.47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1279,7 +1281,7 @@
         <v>28.87</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1296,7 +1298,7 @@
         <v>26.17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1313,7 +1315,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1330,7 +1332,7 @@
         <v>68.569999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>67.760000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1364,7 +1366,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1381,7 +1383,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1398,7 +1400,7 @@
         <v>61.1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1415,7 +1417,7 @@
         <v>12.86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1432,7 +1434,7 @@
         <v>36.46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1449,7 +1451,7 @@
         <v>7.64</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -1466,7 +1468,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1483,7 +1485,7 @@
         <v>21.46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1500,7 +1502,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -1517,7 +1519,7 @@
         <v>57.03</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
@@ -1534,7 +1536,7 @@
         <v>70.63</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -1551,7 +1553,7 @@
         <v>55.48</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
@@ -1568,7 +1570,7 @@
         <v>46.59</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>45</v>
       </c>
@@ -1585,7 +1587,7 @@
         <v>37.94</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>214</v>
       </c>
@@ -1602,7 +1604,7 @@
         <v>46.29</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>214</v>
       </c>
@@ -1619,7 +1621,7 @@
         <v>37.630000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>214</v>
       </c>
@@ -1636,7 +1638,7 @@
         <v>28.61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>214</v>
       </c>
@@ -1653,7 +1655,7 @@
         <v>24.39</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>215</v>
       </c>
@@ -1670,7 +1672,7 @@
         <v>23.47</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>215</v>
       </c>
@@ -1687,7 +1689,7 @@
         <v>7.96</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>215</v>
       </c>
@@ -1704,7 +1706,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>215</v>
       </c>
@@ -1721,7 +1723,7 @@
         <v>6.58</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>215</v>
       </c>
@@ -1738,7 +1740,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>215</v>
       </c>
@@ -1755,7 +1757,7 @@
         <v>46.61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>62</v>
       </c>
@@ -1772,7 +1774,7 @@
         <v>89.8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>62</v>
       </c>
@@ -1789,7 +1791,7 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>65</v>
       </c>
@@ -1806,7 +1808,7 @@
         <v>53.47</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
@@ -1823,7 +1825,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>67</v>
       </c>
@@ -1840,7 +1842,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
@@ -1857,7 +1859,7 @@
         <v>51.13</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>41.65</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>67</v>
       </c>
@@ -1891,7 +1893,7 @@
         <v>21.13</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
@@ -1908,7 +1910,7 @@
         <v>28.27</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>67</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>13.71</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>67</v>
       </c>
@@ -1942,7 +1944,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>67</v>
       </c>
@@ -1959,7 +1961,7 @@
         <v>6.83</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
@@ -1976,7 +1978,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>67</v>
       </c>
@@ -1993,7 +1995,7 @@
         <v>9.8800000000000008</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>67</v>
       </c>
@@ -2010,7 +2012,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>67</v>
       </c>
@@ -2027,7 +2029,7 @@
         <v>6.51</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
@@ -2044,7 +2046,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>67</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>7.87</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>67</v>
       </c>
@@ -2078,7 +2080,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>89</v>
       </c>
@@ -2095,7 +2097,7 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>89</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>89</v>
       </c>
@@ -2129,7 +2131,7 @@
         <v>60.93</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>89</v>
       </c>
@@ -2146,7 +2148,7 @@
         <v>45.74</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>89</v>
       </c>
@@ -2163,7 +2165,7 @@
         <v>30.71</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>89</v>
       </c>
@@ -2180,7 +2182,7 @@
         <v>16.96</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>89</v>
       </c>
@@ -2197,7 +2199,7 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>89</v>
       </c>
@@ -2214,7 +2216,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>89</v>
       </c>
@@ -2231,7 +2233,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>89</v>
       </c>
@@ -2248,7 +2250,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>89</v>
       </c>
@@ -2265,7 +2267,7 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>89</v>
       </c>
@@ -2282,7 +2284,7 @@
         <v>24.06</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>89</v>
       </c>
@@ -2299,7 +2301,7 @@
         <v>13.11</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>89</v>
       </c>
@@ -2316,7 +2318,7 @@
         <v>14.12</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>89</v>
       </c>
@@ -2333,7 +2335,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>105</v>
       </c>
@@ -2350,7 +2352,7 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>105</v>
       </c>
@@ -2367,7 +2369,7 @@
         <v>2.64</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>105</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>40.72</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>105</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>32.82</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>105</v>
       </c>
@@ -2418,7 +2420,7 @@
         <v>17.46</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>105</v>
       </c>
@@ -2435,7 +2437,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>105</v>
       </c>
@@ -2452,7 +2454,7 @@
         <v>2.14</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>105</v>
       </c>
@@ -2469,7 +2471,7 @@
         <v>13.76</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>105</v>
       </c>
@@ -2486,7 +2488,7 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>105</v>
       </c>
@@ -2503,7 +2505,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>105</v>
       </c>
@@ -2520,7 +2522,7 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>105</v>
       </c>
@@ -2537,7 +2539,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>105</v>
       </c>
@@ -2554,7 +2556,7 @@
         <v>14.27</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>105</v>
       </c>
@@ -2571,7 +2573,7 @@
         <v>4.28</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>118</v>
       </c>
@@ -2588,7 +2590,7 @@
         <v>14.27</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>118</v>
       </c>
@@ -2605,7 +2607,7 @@
         <v>37.729999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>118</v>
       </c>
@@ -2622,7 +2624,7 @@
         <v>8.23</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>216</v>
       </c>
@@ -2639,7 +2641,7 @@
         <v>58.39</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>216</v>
       </c>
@@ -2656,7 +2658,7 @@
         <v>29.07</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>217</v>
       </c>
@@ -2673,7 +2675,7 @@
         <v>55.01</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>217</v>
       </c>
@@ -2690,7 +2692,7 @@
         <v>36.28</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>121</v>
       </c>
@@ -2707,7 +2709,7 @@
         <v>14.02</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>121</v>
       </c>
@@ -2724,7 +2726,7 @@
         <v>11.27</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>121</v>
       </c>
@@ -2741,7 +2743,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>121</v>
       </c>
@@ -2758,7 +2760,7 @@
         <v>5.62</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>121</v>
       </c>
@@ -2775,7 +2777,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>121</v>
       </c>
@@ -2792,7 +2794,7 @@
         <v>3.39</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>121</v>
       </c>
@@ -2809,7 +2811,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>218</v>
       </c>
@@ -2826,7 +2828,7 @@
         <v>35.770000000000003</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>218</v>
       </c>
@@ -2843,7 +2845,7 @@
         <v>33.35</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>130</v>
       </c>
@@ -2860,7 +2862,7 @@
         <v>22.09</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>130</v>
       </c>
@@ -2877,7 +2879,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>130</v>
       </c>
@@ -2894,7 +2896,7 @@
         <v>38.54</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>130</v>
       </c>
@@ -2911,7 +2913,7 @@
         <v>14.68</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>130</v>
       </c>
@@ -2928,7 +2930,7 @@
         <v>14.59</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>172</v>
       </c>
@@ -2945,7 +2947,7 @@
         <v>44.53</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>172</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>7.64</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>172</v>
       </c>
@@ -2979,7 +2981,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>174</v>
       </c>
@@ -2996,7 +2998,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>174</v>
       </c>
@@ -3013,7 +3015,7 @@
         <v>12.81</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>174</v>
       </c>
@@ -3030,7 +3032,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>174</v>
       </c>
@@ -3047,7 +3049,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>178</v>
       </c>
@@ -3064,7 +3066,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>178</v>
       </c>
@@ -3081,7 +3083,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>180</v>
       </c>
@@ -3098,7 +3100,7 @@
         <v>58.02</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>180</v>
       </c>
@@ -3115,7 +3117,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>219</v>
       </c>
@@ -3132,7 +3134,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>219</v>
       </c>
@@ -3149,7 +3151,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>219</v>
       </c>
@@ -3166,7 +3168,7 @@
         <v>13.66</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>219</v>
       </c>
@@ -3183,7 +3185,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>219</v>
       </c>
@@ -3200,7 +3202,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>219</v>
       </c>
@@ -3217,7 +3219,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>219</v>
       </c>
@@ -3234,7 +3236,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>219</v>
       </c>
@@ -3251,7 +3253,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>219</v>
       </c>
@@ -3268,7 +3270,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>219</v>
       </c>
@@ -3285,7 +3287,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>219</v>
       </c>
@@ -3302,7 +3304,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>219</v>
       </c>
@@ -3319,7 +3321,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>219</v>
       </c>
@@ -3336,7 +3338,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>219</v>
       </c>
@@ -3353,7 +3355,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>219</v>
       </c>
@@ -3370,7 +3372,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>219</v>
       </c>
@@ -3387,7 +3389,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>219</v>
       </c>
@@ -3404,7 +3406,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>219</v>
       </c>
@@ -3421,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>219</v>
       </c>
@@ -3438,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>219</v>
       </c>
@@ -3455,7 +3457,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>219</v>
       </c>
@@ -3472,7 +3474,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>219</v>
       </c>
@@ -3489,7 +3491,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>219</v>
       </c>
@@ -3506,7 +3508,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>219</v>
       </c>
@@ -3523,7 +3525,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>219</v>
       </c>
@@ -3540,7 +3542,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>219</v>
       </c>
@@ -3557,7 +3559,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>219</v>
       </c>
@@ -3574,7 +3576,7 @@
         <v>13.31</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>219</v>
       </c>
@@ -3591,7 +3593,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>219</v>
       </c>
@@ -3608,7 +3610,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>219</v>
       </c>
@@ -3625,7 +3627,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>219</v>
       </c>
@@ -3642,7 +3644,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>219</v>
       </c>
@@ -3659,7 +3661,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>219</v>
       </c>
@@ -3676,7 +3678,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>219</v>
       </c>
@@ -3693,7 +3695,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>219</v>
       </c>
@@ -3710,7 +3712,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>219</v>
       </c>
@@ -3727,7 +3729,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>219</v>
       </c>
@@ -3744,7 +3746,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>183</v>
       </c>
@@ -3761,7 +3763,7 @@
         <v>92.54</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>183</v>
       </c>
@@ -3778,7 +3780,7 @@
         <v>13.96</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>183</v>
       </c>
@@ -3795,7 +3797,7 @@
         <v>12.29</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>183</v>
       </c>
@@ -3812,7 +3814,7 @@
         <v>30.18</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>183</v>
       </c>
@@ -3829,7 +3831,7 @@
         <v>39.450000000000003</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>183</v>
       </c>
@@ -3846,7 +3848,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>183</v>
       </c>
@@ -3863,7 +3865,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>183</v>
       </c>
@@ -3880,7 +3882,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>183</v>
       </c>
@@ -3897,7 +3899,7 @@
         <v>51.92</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>183</v>
       </c>
@@ -3914,7 +3916,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>194</v>
       </c>
@@ -3931,7 +3933,7 @@
         <v>5.89</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>196</v>
       </c>
@@ -3948,7 +3950,7 @@
         <v>13.59</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>198</v>
       </c>
@@ -3965,7 +3967,7 @@
         <v>38.42</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>198</v>
       </c>
@@ -3982,7 +3984,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>198</v>
       </c>
@@ -3999,7 +4001,7 @@
         <v>14.27</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>198</v>
       </c>
@@ -4016,7 +4018,7 @@
         <v>37.76</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>198</v>
       </c>
@@ -4033,7 +4035,7 @@
         <v>21.99</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>203</v>
       </c>
@@ -4050,7 +4052,7 @@
         <v>12.07</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>203</v>
       </c>
@@ -4067,7 +4069,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>203</v>
       </c>
@@ -4084,7 +4086,7 @@
         <v>62.23</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>203</v>
       </c>
@@ -4101,7 +4103,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>203</v>
       </c>
@@ -4118,7 +4120,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>203</v>
       </c>
@@ -4135,7 +4137,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>203</v>
       </c>
@@ -4152,7 +4154,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>203</v>
       </c>
@@ -4169,7 +4171,7 @@
         <v>17.86</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>203</v>
       </c>
@@ -4187,6 +4189,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E180" xr:uid="{5417913A-0891-445A-91B9-26EAB1278E71}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Breast"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4197,7 +4206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4211,7 +4220,7 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4225,9 +4234,9 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4244,7 +4253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4261,7 +4270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4278,7 +4287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4295,7 +4304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -4312,7 +4321,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4329,7 +4338,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4346,7 +4355,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4363,7 +4372,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -4380,7 +4389,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4397,7 +4406,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -4414,7 +4423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -4431,7 +4440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -4448,7 +4457,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -4465,7 +4474,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -4482,7 +4491,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -4499,7 +4508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -4516,7 +4525,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -4533,7 +4542,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -4550,7 +4559,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -4567,7 +4576,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -4584,7 +4593,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -4601,7 +4610,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -4618,7 +4627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -4635,7 +4644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -4652,7 +4661,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -4669,7 +4678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -4686,7 +4695,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -4703,7 +4712,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -4720,7 +4729,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -4737,7 +4746,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -4754,7 +4763,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -4771,7 +4780,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -4788,7 +4797,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -4805,7 +4814,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -4822,7 +4831,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -4839,7 +4848,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -4856,7 +4865,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -4873,7 +4882,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -4890,7 +4899,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -4907,7 +4916,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -4924,7 +4933,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -4941,7 +4950,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -4958,7 +4967,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -4975,7 +4984,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -4992,7 +5001,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -5009,7 +5018,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -5026,7 +5035,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -5043,7 +5052,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -5060,7 +5069,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -5077,7 +5086,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -5094,7 +5103,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -5111,7 +5120,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -5128,7 +5137,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -5145,7 +5154,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -5162,7 +5171,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -5179,7 +5188,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -5196,7 +5205,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -5213,7 +5222,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -5230,7 +5239,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -5247,7 +5256,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -5264,7 +5273,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -5281,7 +5290,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -5298,7 +5307,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -5315,7 +5324,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -5332,7 +5341,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -5349,7 +5358,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -5366,7 +5375,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -5383,7 +5392,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -5400,7 +5409,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -5417,7 +5426,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -5434,7 +5443,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -5451,7 +5460,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -5468,7 +5477,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -5485,7 +5494,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -5502,7 +5511,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -5519,7 +5528,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -5536,7 +5545,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -5553,7 +5562,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -5570,7 +5579,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -5587,7 +5596,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -5604,7 +5613,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -5621,7 +5630,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -5638,7 +5647,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -5655,7 +5664,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -5672,7 +5681,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -5689,7 +5698,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -5706,7 +5715,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -5723,7 +5732,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -5740,7 +5749,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -5757,7 +5766,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -5774,7 +5783,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -5791,7 +5800,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -5808,7 +5817,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -5825,7 +5834,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -5842,7 +5851,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>5</v>
       </c>
@@ -5859,7 +5868,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -5876,7 +5885,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>5</v>
       </c>
@@ -5893,7 +5902,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -5910,7 +5919,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>5</v>
       </c>
@@ -5927,7 +5936,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>5</v>
       </c>
@@ -5944,7 +5953,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -5961,7 +5970,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -5978,7 +5987,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>5</v>
       </c>
@@ -5995,7 +6004,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>5</v>
       </c>
@@ -6012,7 +6021,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>5</v>
       </c>
@@ -6029,7 +6038,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -6046,7 +6055,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>5</v>
       </c>
@@ -6063,7 +6072,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>5</v>
       </c>
@@ -6080,7 +6089,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>5</v>
       </c>
@@ -6097,7 +6106,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -6114,7 +6123,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -6131,7 +6140,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>5</v>
       </c>
@@ -6148,7 +6157,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>5</v>
       </c>
@@ -6165,7 +6174,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>5</v>
       </c>
@@ -6182,7 +6191,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -6199,7 +6208,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>5</v>
       </c>
@@ -6216,7 +6225,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>5</v>
       </c>
@@ -6233,7 +6242,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>5</v>
       </c>
@@ -6250,7 +6259,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>5</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>5</v>
       </c>
@@ -6284,7 +6293,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>5</v>
       </c>
@@ -6301,7 +6310,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>5</v>
       </c>
@@ -6318,7 +6327,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>5</v>
       </c>
@@ -6335,7 +6344,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>5</v>
       </c>
@@ -6352,7 +6361,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>5</v>
       </c>
@@ -6369,7 +6378,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>5</v>
       </c>
@@ -6386,7 +6395,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>5</v>
       </c>
@@ -6403,7 +6412,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>5</v>
       </c>
@@ -6420,7 +6429,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>5</v>
       </c>
@@ -6437,7 +6446,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>5</v>
       </c>
@@ -6454,7 +6463,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>5</v>
       </c>
@@ -6471,7 +6480,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>5</v>
       </c>
@@ -6488,7 +6497,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>5</v>
       </c>
@@ -6505,7 +6514,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>5</v>
       </c>
@@ -6522,7 +6531,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>5</v>
       </c>
@@ -6539,7 +6548,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>5</v>
       </c>
@@ -6556,7 +6565,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>5</v>
       </c>
@@ -6573,7 +6582,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>5</v>
       </c>
@@ -6590,7 +6599,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>5</v>
       </c>
@@ -6607,7 +6616,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>5</v>
       </c>
@@ -6624,7 +6633,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>5</v>
       </c>
@@ -6641,7 +6650,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>5</v>
       </c>
@@ -6658,7 +6667,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>5</v>
       </c>
@@ -6675,7 +6684,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>5</v>
       </c>
@@ -6692,7 +6701,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>5</v>
       </c>
@@ -6709,7 +6718,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -6726,7 +6735,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>5</v>
       </c>
@@ -6743,7 +6752,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>5</v>
       </c>
@@ -6760,7 +6769,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>5</v>
       </c>
@@ -6777,7 +6786,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>5</v>
       </c>
@@ -6794,7 +6803,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>5</v>
       </c>
@@ -6811,7 +6820,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>5</v>
       </c>
@@ -6828,7 +6837,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>5</v>
       </c>
@@ -6845,7 +6854,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>5</v>
       </c>
@@ -6862,7 +6871,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>5</v>
       </c>
@@ -6879,7 +6888,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>5</v>
       </c>
@@ -6896,7 +6905,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>5</v>
       </c>
@@ -6913,7 +6922,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>5</v>
       </c>
@@ -6930,7 +6939,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>5</v>
       </c>
@@ -6947,7 +6956,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>5</v>
       </c>
@@ -6964,7 +6973,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>5</v>
       </c>
@@ -6981,7 +6990,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>5</v>
       </c>
@@ -6998,7 +7007,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>5</v>
       </c>
@@ -7015,7 +7024,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>5</v>
       </c>
@@ -7032,7 +7041,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>5</v>
       </c>
@@ -7049,7 +7058,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>5</v>
       </c>
@@ -7066,7 +7075,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>5</v>
       </c>
@@ -7083,7 +7092,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>5</v>
       </c>
@@ -7100,7 +7109,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>5</v>
       </c>
@@ -7117,7 +7126,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>5</v>
       </c>
@@ -7134,7 +7143,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
GeneCardv2: changed made to the GeneRiskGraph, Gene is fixed at centre, Cancers labels switch sides depending on where the node is rendered. Embedded the gender option into the graph. Add worked on styling
</commit_message>
<xml_diff>
--- a/data-graph-MUSC/MASTER_RiskTo85ForGraph.xlsx
+++ b/data-graph-MUSC/MASTER_RiskTo85ForGraph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zach/src/_-MUSC/graph-musc/data-graph-MUSC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF82CFB4-A459-9748-8F03-3F6F14BC4A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5D9C5A-E28C-1A48-8362-A8CE40E919DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="500" windowWidth="23900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MASTER_RiskTo85ForGraph!$A$1:$E$180</definedName>
     <definedName name="MASTER_RiskTo85ForGraph">Wrong_MASTER_RiskTo85ForGraph!$A$1:$E$172</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1124,7 +1137,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F191" sqref="F191"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1145,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1281,7 +1296,7 @@
         <v>28.87</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1315,7 +1330,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1383,7 +1398,7 @@
         <v>4.82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1400,7 +1415,7 @@
         <v>61.1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1502,7 +1517,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -1655,7 +1670,7 @@
         <v>24.39</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>215</v>
       </c>
@@ -1842,7 +1857,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
@@ -1859,7 +1874,7 @@
         <v>51.13</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
@@ -2811,7 +2826,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>218</v>
       </c>
@@ -2879,7 +2894,7 @@
         <v>16.350000000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>130</v>
       </c>
@@ -2930,7 +2945,7 @@
         <v>14.59</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>172</v>
       </c>
@@ -3151,7 +3166,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>219</v>
       </c>
@@ -3168,7 +3183,7 @@
         <v>13.66</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>219</v>
       </c>
@@ -3185,7 +3200,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>219</v>
       </c>
@@ -3202,7 +3217,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>219</v>
       </c>
@@ -3746,7 +3761,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>183</v>
       </c>
@@ -3950,7 +3965,7 @@
         <v>13.59</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>198</v>
       </c>
@@ -4069,7 +4084,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>203</v>
       </c>
@@ -4190,9 +4205,15 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E180" xr:uid="{5417913A-0891-445A-91B9-26EAB1278E71}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="MLH1"/>
+        <filter val="Population"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="Breast"/>
+        <filter val="Colorectal"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>